<commit_message>
more model runs and figures for manuscript
</commit_message>
<xml_diff>
--- a/modeling headway FA22/manuscript figs/full model, instant hillslopes, 16 runs + default/phillips figure/sensitivity analysis runs_new.xlsx
+++ b/modeling headway FA22/manuscript figs/full model, instant hillslopes, 16 runs + default/phillips figure/sensitivity analysis runs_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/High-Plains/modeling headway FA22/manuscript figs/full model, instant hillslopes, 16 runs + default/phillips figure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0491AC-53F1-594D-B3AE-FA4668D5C57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC86014-2ABB-A84B-9FED-1AA56EB32625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="500" windowWidth="37420" windowHeight="17660" xr2:uid="{A1E789AD-8EFF-F041-AF6E-58597918FEEE}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{A1E789AD-8EFF-F041-AF6E-58597918FEEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5207919-DF38-274C-BB08-71501418D0F8}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
all progress up to BIGANTR submission
</commit_message>
<xml_diff>
--- a/modeling headway FA22/manuscript figs/full model, instant hillslopes, 16 runs + default/phillips figure/sensitivity analysis runs_new.xlsx
+++ b/modeling headway FA22/manuscript figs/full model, instant hillslopes, 16 runs + default/phillips figure/sensitivity analysis runs_new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/High-Plains/modeling headway FA22/manuscript figs/full model, instant hillslopes, 16 runs + default/phillips figure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC86014-2ABB-A84B-9FED-1AA56EB32625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFB29BC-68BA-A747-8C2A-0A5A18433912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{A1E789AD-8EFF-F041-AF6E-58597918FEEE}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,7 +792,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="H5" s="2">
-        <v>5.0000000000000001E-4</v>
+        <v>5</v>
       </c>
       <c r="I5" s="2">
         <v>4.1000000000000002E-2</v>

</xml_diff>